<commit_message>
Finalised SessionUpload. Added accessions copy script.
</commit_message>
<xml_diff>
--- a/Library/Templates/test_checklist.small.xlsx
+++ b/Library/Templates/test_checklist.small.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="724" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="724"/>
   </bookViews>
   <sheets>
     <sheet name="CK_Identification" sheetId="10" r:id="rId1"/>
@@ -2245,9 +2245,9 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AS16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA8" sqref="AA8"/>
+      <selection pane="bottomLeft" activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3874,7 +3874,7 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>

</xml_diff>

<commit_message>
Fixed a bug in ExcelTemplateParser: it would add the related worksheet and field even if the relation field was not provided. Fixed a bug in SessionUpdate, typo. Renamed in standards templates symbol CK_UNID in UNID, to have one element. Updated test and official templates for the above change.
</commit_message>
<xml_diff>
--- a/Library/Templates/test_checklist.small.xlsx
+++ b/Library/Templates/test_checklist.small.xlsx
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>Checklist identifier</t>
-  </si>
-  <si>
-    <t>Field specific for uniquely identifying your cwr checklist. The combination you provide must be unique for each row on the first column of the excel worksheet.</t>
-  </si>
-  <si>
-    <t>CK_UNID</t>
   </si>
   <si>
     <t>Dataset</t>
@@ -1271,14 +1265,27 @@
   <si>
     <t>Difficult</t>
   </si>
+  <si>
+    <t>Field specific for uniquely identifying your checklist. The combination you provide must be unique for each row on the first column of the excel worksheet.</t>
+  </si>
+  <si>
+    <t>UNID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1378,8 +1385,16 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1402,6 +1417,18 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD5B4"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1553,121 +1580,122 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="110">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1687,31 +1715,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1720,21 +1748,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1743,88 +1771,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="105" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="105" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="105" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="105" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1832,8 +1860,32 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="110">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1890,6 +1942,7 @@
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2247,7 +2300,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS13" sqref="AS13"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2311,10 +2364,10 @@
       <c r="A2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -2358,10 +2411,10 @@
     </row>
     <row r="3" spans="1:45" s="11" customFormat="1" ht="15">
       <c r="A3" s="26"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -2407,181 +2460,181 @@
       <c r="A4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="K4" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="G4" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="J4" s="18" t="s">
+      <c r="L4" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="45" t="s">
-        <v>36</v>
-      </c>
       <c r="O4" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="T4" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="X4" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q4" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="S4" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="T4" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="V4" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="W4" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="X4" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y4" s="43" t="s">
-        <v>41</v>
-      </c>
       <c r="Z4" s="43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AA4" s="43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AB4" s="43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC4" s="43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AD4" s="43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AE4" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF4" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="AF4" s="43" t="s">
-        <v>88</v>
-      </c>
       <c r="AG4" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH4" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="AH4" s="43" t="s">
+      <c r="AI4" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="AI4" s="43" t="s">
+      <c r="AJ4" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK4" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL4" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM4" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN4" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="AO4" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="AP4" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ4" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="AJ4" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK4" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL4" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="AM4" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="AN4" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="AO4" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP4" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="AQ4" s="43" t="s">
-        <v>97</v>
-      </c>
       <c r="AR4" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS4" s="46" t="s">
         <v>100</v>
-      </c>
-      <c r="AS4" s="46" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:45" s="7" customFormat="1" ht="154">
       <c r="A5" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="68" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="53" t="s">
-        <v>143</v>
+      <c r="E5" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>149</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>152</v>
+        <v>144</v>
+      </c>
+      <c r="H5" s="53" t="s">
+        <v>147</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J5" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
@@ -2589,43 +2642,43 @@
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
       <c r="T5" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U5" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V5" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X5" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Y5" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Z5" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AA5" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AB5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="AC5" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AD5" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AE5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="AF5" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AG5" s="13" t="s">
         <v>8</v>
@@ -2637,59 +2690,59 @@
         <v>9</v>
       </c>
       <c r="AJ5" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AK5" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AL5" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AM5" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AN5" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AO5" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AP5" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AQ5" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AR5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="AS5" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:45" s="8" customFormat="1" ht="70">
       <c r="A6" s="31"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54" t="s">
-        <v>23</v>
-      </c>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="54"/>
       <c r="G6" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>29</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N6" s="14">
         <v>2</v>
@@ -2710,35 +2763,35 @@
         <v>5</v>
       </c>
       <c r="T6" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V6" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="W6" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="X6" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Y6" s="15"/>
       <c r="Z6" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AA6" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AB6" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AC6" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AD6" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AE6" s="22"/>
       <c r="AF6" s="22"/>
@@ -2746,17 +2799,17 @@
       <c r="AH6" s="22"/>
       <c r="AI6" s="22"/>
       <c r="AJ6" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AK6" s="22"/>
       <c r="AL6" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AM6" s="22"/>
       <c r="AN6" s="22"/>
       <c r="AO6" s="22"/>
       <c r="AP6" s="22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AQ6" s="22"/>
       <c r="AR6" s="22"/>
@@ -2764,32 +2817,32 @@
     </row>
     <row r="7" spans="1:45" s="8" customFormat="1">
       <c r="A7" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="55"/>
+        <v>22</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="72" t="s">
+        <v>28</v>
+      </c>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
-      <c r="H7" s="16"/>
+      <c r="H7" s="55"/>
       <c r="I7" s="16"/>
-      <c r="J7" s="17" t="s">
-        <v>30</v>
-      </c>
+      <c r="J7" s="16"/>
       <c r="K7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
@@ -2797,18 +2850,18 @@
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
       <c r="T7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="U7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="V7" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W7" s="16"/>
       <c r="X7" s="17"/>
       <c r="Y7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Z7" s="16"/>
       <c r="AA7" s="16"/>
@@ -2833,139 +2886,139 @@
     </row>
     <row r="8" spans="1:45" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="A8" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>141</v>
+        <v>334</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="71" t="s">
+        <v>131</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>151</v>
+        <v>143</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>146</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L8" s="36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="36" t="s">
-        <v>40</v>
-      </c>
       <c r="P8" s="36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q8" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="R8" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="R8" s="37" t="s">
-        <v>48</v>
-      </c>
       <c r="S8" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T8" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U8" s="37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V8" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="W8" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="X8" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="X8" s="37" t="s">
-        <v>69</v>
-      </c>
       <c r="Y8" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Z8" s="36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AA8" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AB8" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AC8" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AD8" s="37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AE8" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF8" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="AF8" s="37" t="s">
-        <v>89</v>
-      </c>
       <c r="AG8" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH8" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="AH8" s="37" t="s">
+      <c r="AI8" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="AI8" s="37" t="s">
+      <c r="AJ8" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK8" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL8" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM8" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN8" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO8" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP8" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ8" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="AJ8" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK8" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL8" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM8" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="AN8" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="AO8" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP8" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="AQ8" s="37" t="s">
-        <v>98</v>
-      </c>
       <c r="AR8" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS8" s="38" t="s">
         <v>101</v>
-      </c>
-      <c r="AS8" s="38" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:45" ht="28">
@@ -2973,262 +3026,262 @@
         <v>1</v>
       </c>
       <c r="B9" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="C9" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="D9" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="E9" s="60"/>
+      <c r="E9" s="61" t="s">
+        <v>261</v>
+      </c>
       <c r="F9" s="60"/>
       <c r="G9" s="60"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="59" t="s">
-        <v>273</v>
-      </c>
-      <c r="J9" s="61" t="s">
-        <v>263</v>
+      <c r="H9" s="60"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59" t="s">
+        <v>271</v>
       </c>
       <c r="K9" s="58" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L9" s="58">
         <v>201503</v>
       </c>
       <c r="M9" s="58" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N9" s="58">
         <v>2</v>
       </c>
       <c r="O9" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="P9" s="58" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q9" s="58" t="s">
+        <v>273</v>
+      </c>
+      <c r="R9" s="58" t="s">
+        <v>274</v>
+      </c>
+      <c r="S9" s="58" t="s">
+        <v>275</v>
+      </c>
+      <c r="T9" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="U9" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="P9" s="58" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q9" s="58" t="s">
-        <v>275</v>
-      </c>
-      <c r="R9" s="58" t="s">
+      <c r="V9" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="W9" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="X9" s="58" t="s">
         <v>276</v>
       </c>
-      <c r="S9" s="58" t="s">
+      <c r="Y9" s="58" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z9" s="58" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA9" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB9" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC9" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD9" s="58" t="s">
         <v>277</v>
       </c>
-      <c r="T9" s="58" t="s">
-        <v>245</v>
-      </c>
-      <c r="U9" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="V9" s="58" t="s">
-        <v>247</v>
-      </c>
-      <c r="W9" s="58" t="s">
-        <v>248</v>
-      </c>
-      <c r="X9" s="58" t="s">
+      <c r="AE9" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF9" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="Y9" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z9" s="58" t="s">
-        <v>250</v>
-      </c>
-      <c r="AA9" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB9" s="58" t="s">
+      <c r="AG9" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH9" s="58" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI9" s="58" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ9" s="60" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK9" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL9" s="60" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM9" s="58" t="s">
+        <v>285</v>
+      </c>
+      <c r="AN9" s="60" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO9" s="60" t="s">
         <v>252</v>
-      </c>
-      <c r="AC9" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD9" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE9" s="58" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF9" s="58" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG9" s="58" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH9" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI9" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="AJ9" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK9" s="58" t="s">
-        <v>285</v>
-      </c>
-      <c r="AL9" s="60" t="s">
-        <v>286</v>
-      </c>
-      <c r="AM9" s="58" t="s">
-        <v>287</v>
-      </c>
-      <c r="AN9" s="60" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO9" s="60" t="s">
-        <v>254</v>
       </c>
       <c r="AP9" s="60">
         <v>30</v>
       </c>
       <c r="AQ9" s="60" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AR9" s="60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AS9" s="60" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:45" ht="28">
       <c r="B10" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C10" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E10"/>
+      <c r="E10" s="51" t="s">
+        <v>261</v>
+      </c>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="I10" s="50" t="s">
-        <v>273</v>
-      </c>
-      <c r="J10" s="51" t="s">
-        <v>263</v>
+      <c r="H10"/>
+      <c r="J10" s="50" t="s">
+        <v>271</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L10" s="5">
         <v>201503</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N10" s="5">
         <v>2</v>
       </c>
       <c r="O10" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="U10" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="P10" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="R10" s="5" t="s">
+      <c r="V10" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="X10" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S10" s="5" t="s">
+      <c r="Y10" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD10" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="T10" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="V10" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="W10" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="X10" s="5" t="s">
+      <c r="AE10" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF10" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="Y10" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="AA10" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB10" s="5" t="s">
+      <c r="AG10" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI10" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK10" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO10" t="s">
         <v>252</v>
-      </c>
-      <c r="AC10" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD10" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE10" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF10" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG10" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH10" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI10" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK10" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>286</v>
-      </c>
-      <c r="AM10" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>254</v>
       </c>
       <c r="AP10">
         <v>30</v>
       </c>
       <c r="AQ10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AR10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AS10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:45">
       <c r="C11" s="50"/>
-      <c r="E11"/>
+      <c r="E11" s="51"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="51"/>
+      <c r="H11"/>
+      <c r="J11" s="50"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="5"/>
       <c r="AG11" s="5"/>
@@ -3242,127 +3295,127 @@
         <v>3</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E12"/>
+      <c r="E12" s="51" t="s">
+        <v>261</v>
+      </c>
       <c r="F12"/>
       <c r="G12"/>
-      <c r="I12" s="50" t="s">
-        <v>273</v>
-      </c>
-      <c r="J12" s="51" t="s">
-        <v>263</v>
+      <c r="H12"/>
+      <c r="J12" s="50" t="s">
+        <v>271</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L12" s="5">
         <v>201503</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N12" s="5">
         <v>2</v>
       </c>
       <c r="O12" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="U12" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="P12" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="R12" s="5" t="s">
+      <c r="V12" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="X12" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="Y12" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD12" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="T12" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="U12" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="V12" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="W12" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="X12" s="5" t="s">
+      <c r="AE12" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF12" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="Y12" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z12" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="AA12" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB12" s="5" t="s">
+      <c r="AG12" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH12" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI12" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK12" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM12" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO12" t="s">
         <v>252</v>
-      </c>
-      <c r="AC12" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD12" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE12" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF12" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG12" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH12" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI12" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK12" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>286</v>
-      </c>
-      <c r="AM12" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>254</v>
       </c>
       <c r="AP12">
         <v>30</v>
       </c>
       <c r="AQ12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AR12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AS12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:45" ht="28">
@@ -3370,128 +3423,128 @@
         <v>4</v>
       </c>
       <c r="B13" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="D13" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="C13" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="D13" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="E13" s="60"/>
+      <c r="E13" s="61" t="s">
+        <v>261</v>
+      </c>
       <c r="F13" s="60"/>
       <c r="G13" s="60"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="59" t="s">
-        <v>273</v>
-      </c>
-      <c r="J13" s="61" t="s">
-        <v>263</v>
+      <c r="H13" s="60"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="59" t="s">
+        <v>271</v>
       </c>
       <c r="K13" s="58" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L13" s="58">
         <v>201503</v>
       </c>
       <c r="M13" s="58" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N13" s="58">
         <v>2</v>
       </c>
       <c r="O13" s="58" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="P13" s="58" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q13" s="58" t="s">
+        <v>273</v>
+      </c>
+      <c r="R13" s="58" t="s">
         <v>274</v>
       </c>
-      <c r="Q13" s="58" t="s">
+      <c r="S13" s="58" t="s">
         <v>275</v>
       </c>
-      <c r="R13" s="58" t="s">
-        <v>276</v>
-      </c>
-      <c r="S13" s="58" t="s">
+      <c r="T13" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="U13" s="58" t="s">
+        <v>296</v>
+      </c>
+      <c r="V13" s="58" t="s">
+        <v>297</v>
+      </c>
+      <c r="W13" s="58" t="s">
+        <v>298</v>
+      </c>
+      <c r="X13" s="58" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y13" s="58" t="s">
+        <v>300</v>
+      </c>
+      <c r="Z13" s="59" t="s">
+        <v>301</v>
+      </c>
+      <c r="AA13" s="58" t="s">
+        <v>302</v>
+      </c>
+      <c r="AB13" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC13" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD13" s="58" t="s">
         <v>277</v>
       </c>
-      <c r="T13" s="58" t="s">
-        <v>293</v>
-      </c>
-      <c r="U13" s="58" t="s">
-        <v>298</v>
-      </c>
-      <c r="V13" s="58" t="s">
-        <v>299</v>
-      </c>
-      <c r="W13" s="58" t="s">
-        <v>300</v>
-      </c>
-      <c r="X13" s="58" t="s">
-        <v>301</v>
-      </c>
-      <c r="Y13" s="58" t="s">
-        <v>302</v>
-      </c>
-      <c r="Z13" s="59" t="s">
+      <c r="AE13" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF13" s="58" t="s">
+        <v>278</v>
+      </c>
+      <c r="AG13" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH13" s="58" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI13" s="58" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ13" s="60" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK13" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL13" s="60" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM13" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="AA13" s="58" t="s">
-        <v>304</v>
-      </c>
-      <c r="AB13" s="58" t="s">
+      <c r="AN13" s="60" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO13" s="60" t="s">
         <v>252</v>
-      </c>
-      <c r="AC13" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD13" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE13" s="58" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF13" s="58" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG13" s="58" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH13" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI13" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="AJ13" s="60" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK13" s="58" t="s">
-        <v>285</v>
-      </c>
-      <c r="AL13" s="60" t="s">
-        <v>286</v>
-      </c>
-      <c r="AM13" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="AN13" s="60" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO13" s="60" t="s">
-        <v>254</v>
       </c>
       <c r="AP13" s="60">
         <v>30</v>
       </c>
       <c r="AQ13" s="60" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AR13" s="60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AS13" s="60" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:45" ht="28">
@@ -3499,124 +3552,124 @@
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C14" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E14"/>
+      <c r="E14" s="51" t="s">
+        <v>261</v>
+      </c>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="I14" s="50" t="s">
-        <v>273</v>
-      </c>
-      <c r="J14" s="51" t="s">
-        <v>263</v>
+      <c r="H14"/>
+      <c r="J14" s="50" t="s">
+        <v>271</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N14" s="5">
         <v>5</v>
       </c>
       <c r="O14" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="U14" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="P14" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="R14" s="5" t="s">
+      <c r="V14" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="X14" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S14" s="5" t="s">
+      <c r="Y14" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB14" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD14" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="T14" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="V14" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="W14" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="X14" s="5" t="s">
+      <c r="AE14" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF14" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="Y14" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z14" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="AA14" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB14" s="5" t="s">
+      <c r="AG14" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH14" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI14" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK14" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM14" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO14" t="s">
         <v>252</v>
-      </c>
-      <c r="AC14" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD14" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE14" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF14" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG14" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH14" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI14" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK14" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>286</v>
-      </c>
-      <c r="AM14" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>254</v>
       </c>
       <c r="AP14">
         <v>70</v>
       </c>
       <c r="AQ14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AR14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AS14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:45" ht="28">
@@ -3624,109 +3677,109 @@
         <v>6</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C15" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E15"/>
+      <c r="E15" s="51" t="s">
+        <v>261</v>
+      </c>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="I15" s="50" t="s">
+      <c r="H15"/>
+      <c r="J15" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q15" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="J15" s="51" t="s">
-        <v>263</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="P15" s="5" t="s">
+      <c r="R15" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="S15" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="R15" s="5" t="s">
+      <c r="V15" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="W15" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="X15" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S15" s="5" t="s">
+      <c r="Z15" s="50" t="s">
+        <v>306</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD15" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="V15" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="W15" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="X15" s="5" t="s">
+      <c r="AE15" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF15" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="Z15" s="50" t="s">
-        <v>308</v>
-      </c>
-      <c r="AA15" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB15" s="5" t="s">
+      <c r="AG15" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH15" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI15" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK15" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM15" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO15" t="s">
         <v>252</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD15" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF15" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG15" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH15" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI15" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK15" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>286</v>
-      </c>
-      <c r="AM15" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>254</v>
       </c>
       <c r="AP15">
         <v>70</v>
       </c>
       <c r="AQ15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AR15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AS15" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:45" ht="28">
@@ -3734,129 +3787,129 @@
         <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C16" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E16"/>
+      <c r="E16" s="51" t="s">
+        <v>261</v>
+      </c>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="I16" s="50" t="s">
+      <c r="H16"/>
+      <c r="J16" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q16" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="J16" s="51" t="s">
-        <v>263</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="P16" s="5" t="s">
+      <c r="R16" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="Q16" s="5" t="s">
+      <c r="S16" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="R16" s="5" t="s">
+      <c r="V16" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="X16" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S16" s="5" t="s">
+      <c r="Z16" s="50" t="s">
+        <v>306</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD16" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="V16" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="W16" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="X16" s="5" t="s">
+      <c r="AE16" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF16" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="Z16" s="50" t="s">
-        <v>308</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB16" s="5" t="s">
+      <c r="AG16" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH16" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI16" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>282</v>
+      </c>
+      <c r="AK16" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>284</v>
+      </c>
+      <c r="AM16" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO16" t="s">
         <v>252</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF16" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AH16" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="AI16" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>284</v>
-      </c>
-      <c r="AK16" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>286</v>
-      </c>
-      <c r="AM16" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO16" t="s">
-        <v>254</v>
       </c>
       <c r="AP16">
         <v>70</v>
       </c>
       <c r="AQ16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AR16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AS16" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1"/>
-    <hyperlink ref="I9" r:id="rId2" display="http://bioversityinternational.org"/>
+    <hyperlink ref="J9" r:id="rId2" display="http://bioversityinternational.org"/>
     <hyperlink ref="C10" r:id="rId3"/>
     <hyperlink ref="C12" r:id="rId4"/>
     <hyperlink ref="C13" r:id="rId5"/>
     <hyperlink ref="C14" r:id="rId6"/>
-    <hyperlink ref="I10" r:id="rId7" display="http://bioversityinternational.org"/>
-    <hyperlink ref="I12" r:id="rId8" display="http://bioversityinternational.org"/>
-    <hyperlink ref="I13" r:id="rId9" display="http://bioversityinternational.org"/>
-    <hyperlink ref="I14" r:id="rId10" display="http://bioversityinternational.org"/>
+    <hyperlink ref="J10" r:id="rId7" display="http://bioversityinternational.org"/>
+    <hyperlink ref="J12" r:id="rId8" display="http://bioversityinternational.org"/>
+    <hyperlink ref="J13" r:id="rId9" display="http://bioversityinternational.org"/>
+    <hyperlink ref="J14" r:id="rId10" display="http://bioversityinternational.org"/>
     <hyperlink ref="Z13" r:id="rId11"/>
     <hyperlink ref="C15" r:id="rId12"/>
-    <hyperlink ref="I15" r:id="rId13" display="http://bioversityinternational.org"/>
+    <hyperlink ref="J15" r:id="rId13" display="http://bioversityinternational.org"/>
     <hyperlink ref="Z15" r:id="rId14"/>
     <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="I16" r:id="rId16" display="http://bioversityinternational.org"/>
+    <hyperlink ref="J16" r:id="rId16" display="http://bioversityinternational.org"/>
     <hyperlink ref="Z16" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3876,7 +3929,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3888,7 +3941,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3898,7 +3951,7 @@
     </row>
     <row r="2" spans="1:6" ht="15">
       <c r="A2" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -3919,39 +3972,39 @@
         <v>16</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="70">
       <c r="A5" s="29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3964,7 +4017,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -3973,23 +4026,23 @@
       <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1">
-      <c r="A8" s="35" t="s">
-        <v>18</v>
+      <c r="A8" s="73" t="s">
+        <v>334</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="64" customFormat="1">
@@ -3997,19 +4050,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F9" s="58" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="64" customFormat="1">
@@ -4017,19 +4070,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E10" s="58">
         <v>75</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="64" customFormat="1">
@@ -4037,19 +4090,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E11" s="58">
         <v>60</v>
       </c>
       <c r="F11" s="58" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="64" customFormat="1">
@@ -4057,19 +4110,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="58" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>322</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>307</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="F12" s="58" t="s">
         <v>323</v>
-      </c>
-      <c r="C12" s="58" t="s">
-        <v>324</v>
-      </c>
-      <c r="D12" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>334</v>
-      </c>
-      <c r="F12" s="58" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4082,37 +4135,37 @@
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E14" s="5">
         <v>60</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="64" customFormat="1">
       <c r="A15" s="62"/>
       <c r="B15" s="63" t="s">
+        <v>321</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>322</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>307</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>332</v>
+      </c>
+      <c r="F15" s="63" t="s">
         <v>323</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>324</v>
-      </c>
-      <c r="D15" s="63" t="s">
-        <v>309</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>334</v>
-      </c>
-      <c r="F15" s="63" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="64" customFormat="1">
@@ -4120,19 +4173,19 @@
         <v>999</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E16" s="65">
         <v>0.66</v>
       </c>
       <c r="F16" s="63" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -4153,7 +4206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4164,7 +4217,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18">
       <c r="A1" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -4188,7 +4241,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="15">
       <c r="A2" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -4237,150 +4290,150 @@
         <v>16</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C4" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="43" t="s">
-        <v>183</v>
-      </c>
       <c r="E4" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="G4" s="43" t="s">
-        <v>191</v>
-      </c>
       <c r="H4" s="43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K4" s="43" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L4" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M4" s="45" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N4" s="45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O4" s="43" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Q4" s="43" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R4" s="43" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="S4" s="43" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="T4" s="48" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="4" customFormat="1" ht="224">
       <c r="A5" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L5" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="M5" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="M5" s="21" t="s">
-        <v>213</v>
-      </c>
       <c r="N5" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="R5" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="S5" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="S5" s="13" t="s">
-        <v>232</v>
-      </c>
       <c r="T5" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="4" customFormat="1">
       <c r="A6" s="31"/>
       <c r="B6" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N6" s="14"/>
       <c r="O6" s="15"/>
@@ -4388,13 +4441,13 @@
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
       <c r="S6" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="T6" s="49"/>
     </row>
     <row r="7" spans="1:20" s="4" customFormat="1">
       <c r="A7" s="33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -4414,70 +4467,70 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
       <c r="S7" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T7" s="34"/>
     </row>
     <row r="8" spans="1:20" s="3" customFormat="1" ht="15" thickBot="1">
-      <c r="A8" s="35" t="s">
-        <v>18</v>
+      <c r="A8" s="73" t="s">
+        <v>334</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D8" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="G8" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="F8" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="G8" s="36" t="s">
+      <c r="H8" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="H8" s="36" t="s">
-        <v>197</v>
-      </c>
       <c r="I8" s="36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L8" s="36" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N8" s="36" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O8" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="P8" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="P8" s="36" t="s">
-        <v>223</v>
-      </c>
       <c r="Q8" s="36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R8" s="37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="S8" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="T8" s="38" t="s">
         <v>233</v>
-      </c>
-      <c r="T8" s="38" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -4488,22 +4541,22 @@
         <v>2</v>
       </c>
       <c r="C9" s="58" t="s">
+        <v>255</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="F9" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="G9" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="H9" s="58" t="s">
         <v>259</v>
-      </c>
-      <c r="F9" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="G9" s="58" t="s">
-        <v>260</v>
-      </c>
-      <c r="H9" s="58" t="s">
-        <v>261</v>
       </c>
       <c r="I9" s="58">
         <v>2</v>
@@ -4512,25 +4565,25 @@
         <v>2015</v>
       </c>
       <c r="K9" s="59" t="s">
+        <v>311</v>
+      </c>
+      <c r="L9" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="M9" s="58" t="s">
+        <v>260</v>
+      </c>
+      <c r="N9" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="O9" s="58" t="s">
         <v>313</v>
-      </c>
-      <c r="L9" s="58" t="s">
-        <v>314</v>
-      </c>
-      <c r="M9" s="58" t="s">
-        <v>262</v>
-      </c>
-      <c r="N9" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="O9" s="58" t="s">
-        <v>315</v>
       </c>
       <c r="P9" s="58" t="s">
         <v>0</v>
       </c>
       <c r="Q9" s="58" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="R9" s="58">
         <v>1987</v>
@@ -4539,7 +4592,7 @@
         <v>100</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -4550,22 +4603,22 @@
         <v>2</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G10" s="58" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H10" s="58" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I10" s="58">
         <v>3</v>
@@ -4574,25 +4627,25 @@
         <v>2015</v>
       </c>
       <c r="K10" s="59" t="s">
+        <v>311</v>
+      </c>
+      <c r="L10" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="M10" s="58" t="s">
+        <v>260</v>
+      </c>
+      <c r="N10" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="O10" s="58" t="s">
         <v>313</v>
-      </c>
-      <c r="L10" s="58" t="s">
-        <v>314</v>
-      </c>
-      <c r="M10" s="58" t="s">
-        <v>262</v>
-      </c>
-      <c r="N10" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="O10" s="58" t="s">
-        <v>315</v>
       </c>
       <c r="P10" s="58" t="s">
         <v>0</v>
       </c>
       <c r="Q10" s="58" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="R10" s="58">
         <v>1987</v>
@@ -4601,7 +4654,7 @@
         <v>410</v>
       </c>
       <c r="T10" s="58" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -4612,22 +4665,22 @@
         <v>3</v>
       </c>
       <c r="C11" s="58" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>266</v>
+      </c>
+      <c r="E11" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="F11" s="58" t="s">
+        <v>315</v>
+      </c>
+      <c r="G11" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="H11" s="58" t="s">
         <v>269</v>
-      </c>
-      <c r="F11" s="58" t="s">
-        <v>317</v>
-      </c>
-      <c r="G11" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="H11" s="58" t="s">
-        <v>271</v>
       </c>
       <c r="I11" s="58">
         <v>3</v>
@@ -4636,25 +4689,25 @@
         <v>2015</v>
       </c>
       <c r="K11" s="59" t="s">
+        <v>311</v>
+      </c>
+      <c r="L11" s="58" t="s">
+        <v>316</v>
+      </c>
+      <c r="M11" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="N11" s="58" t="s">
+        <v>317</v>
+      </c>
+      <c r="O11" s="58" t="s">
         <v>313</v>
-      </c>
-      <c r="L11" s="58" t="s">
-        <v>318</v>
-      </c>
-      <c r="M11" s="58" t="s">
-        <v>272</v>
-      </c>
-      <c r="N11" s="58" t="s">
-        <v>319</v>
-      </c>
-      <c r="O11" s="58" t="s">
-        <v>315</v>
       </c>
       <c r="P11" s="58" t="s">
         <v>0</v>
       </c>
       <c r="Q11" s="58" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="R11" s="58">
         <v>1977</v>
@@ -4663,7 +4716,7 @@
         <v>410</v>
       </c>
       <c r="T11" s="58" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -4674,22 +4727,22 @@
         <v>3</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D12" s="58" t="s">
+        <v>266</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>267</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>315</v>
+      </c>
+      <c r="G12" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="H12" s="58" t="s">
         <v>269</v>
-      </c>
-      <c r="F12" s="58" t="s">
-        <v>317</v>
-      </c>
-      <c r="G12" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="H12" s="58" t="s">
-        <v>271</v>
       </c>
       <c r="I12" s="58">
         <v>3</v>
@@ -4697,22 +4750,22 @@
       <c r="J12" s="58"/>
       <c r="K12" s="59"/>
       <c r="L12" s="58" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M12" s="58" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="N12" s="58" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="O12" s="58" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P12" s="58" t="s">
         <v>0</v>
       </c>
       <c r="Q12" s="58" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="R12" s="58">
         <v>1977</v>
@@ -4721,7 +4774,7 @@
         <v>410</v>
       </c>
       <c r="T12" s="58" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -4754,19 +4807,19 @@
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>269</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>271</v>
       </c>
       <c r="I14" s="5">
         <v>3</v>
@@ -4775,13 +4828,13 @@
         <v>2015</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="S14" s="5">
         <v>410</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -4792,34 +4845,34 @@
         <v>4</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>330</v>
       </c>
       <c r="I15" s="5">
         <v>4</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -4830,31 +4883,31 @@
         <v>4</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>330</v>
       </c>
       <c r="I16" s="5">
         <v>4</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="2:20">
@@ -4862,34 +4915,34 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>330</v>
       </c>
       <c r="I17" s="5">
         <v>4</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalised template update. Finalised inventory template.
</commit_message>
<xml_diff>
--- a/Library/Templates/test_checklist.small.xlsx
+++ b/Library/Templates/test_checklist.small.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="724"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="724" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CK_Identification" sheetId="10" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="378">
   <si>
     <t>Description</t>
   </si>
@@ -1270,6 +1270,208 @@
   </si>
   <si>
     <t>UNID</t>
+  </si>
+  <si>
+    <t>Reproductive system</t>
+  </si>
+  <si>
+    <t>Breeding system</t>
+  </si>
+  <si>
+    <t>Flower/plant sex structure</t>
+  </si>
+  <si>
+    <t>Pollination</t>
+  </si>
+  <si>
+    <t>Life form</t>
+  </si>
+  <si>
+    <t>Life span</t>
+  </si>
+  <si>
+    <t>Seed dispersal</t>
+  </si>
+  <si>
+    <t>1. Sexual
+2. Vegetative
+Separate multiple entries with a semicolon (;)</t>
+  </si>
+  <si>
+    <t>1. Allogamous
+2. Autogamous
+Separate multiple entries with a semicolon (;)</t>
+  </si>
+  <si>
+    <t>1. Andromonoecious(Plants have some male and hermaphrodite flowers)
+2. Gynodioecious (Plants have female and hermaphrodite flowers)
+3. Dioecious (Having either only male or only female flowers. No individual plant of the population produces both pollen and ovules)
+4. Hermaphrodite (All plants with hermaphrodite flowers)
+Separate multiple entries with a semicolon (;)</t>
+  </si>
+  <si>
+    <t>1. Ants
+2. Bats
+3. Bees
+4. Beetles
+5. Birds
+6. Butterflies
+7. Other insect
+8. Moths
+9. Wind
+Separate multiple entries with a semicolon (;)</t>
+  </si>
+  <si>
+    <t>1. Phanerophytes (phan.) 
+2. Nanophanerophytes (nanophan.) 
+3. Herbaceous phanerophytes (herb. phan.) 
+4. Chamaephytes (cham.) 
+5. Hemicryptophytes (hemicr.) 
+6. Geophytes (not abbreviated) 
+7. Therophytes (ther.) 
+8. Epiphytes (epi.) 
+9. Helophytes (hel.) 
+10. Hydrophytes (hydro.) 
+Separate multiple entries with a semicolon (;)</t>
+  </si>
+  <si>
+    <t>1. Annual
+2. Perennial.
+3. Biennial</t>
+  </si>
+  <si>
+    <t>1. Anemochorous 
+2. Anthropochory 
+3. Endozoochory 
+4. Myrmecochory
+5. Zoochorous 
+Separate multiple entries with a semicolon (;)</t>
+  </si>
+  <si>
+    <t>1
+2
+1;2</t>
+  </si>
+  <si>
+    <t>1
+3</t>
+  </si>
+  <si>
+    <t>3
+6;7</t>
+  </si>
+  <si>
+    <t>5
+2</t>
+  </si>
+  <si>
+    <t>1
+3;5</t>
+  </si>
+  <si>
+    <t>REPSYSTEM</t>
+  </si>
+  <si>
+    <t>BREDSYSTEM</t>
+  </si>
+  <si>
+    <t>SEXSTRUCT</t>
+  </si>
+  <si>
+    <t>POLLINATION</t>
+  </si>
+  <si>
+    <t>LIFEFORM</t>
+  </si>
+  <si>
+    <t>LIFESPAN</t>
+  </si>
+  <si>
+    <t>SEEDDISPERSAL</t>
+  </si>
+  <si>
+    <t>Country of assessment</t>
+  </si>
+  <si>
+    <t>Administrative unit of assessment</t>
+  </si>
+  <si>
+    <r>
+      <t>Provide the ISO code of the country of assessment if level is 3 (= national). Use the three-letter ISO code (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Standard ISO 3166-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>Provide the geographical administrative unit related to the assessment this may be a country or a country subdivision. For country codes use the three-letter ISO 3166-1 Alpha-3 code; for region codes use the ISO 3166-2 codes (see: http://en.wikipedia.org/wiki/ISO_3166-1).</t>
+  </si>
+  <si>
+    <t>ESP for Spain
+GBR for United Kingdom</t>
+  </si>
+  <si>
+    <t>ES-AN for the autonomous community of Andalucía
+GB-SCT for Scotland
+GB-WLS for Wales</t>
+  </si>
+  <si>
+    <t>ASSESSMENT_COUNTRY</t>
+  </si>
+  <si>
+    <t>ASSESSMENT_ADMIN</t>
+  </si>
+  <si>
+    <t>IT-NA</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>GB-SCT</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>ES-AN</t>
+  </si>
+  <si>
+    <t>Biological status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biological status of the threatened species.
+100. Wild
+  110.  Natural
+  120. Semi-natural
+  130. Natural/sown
+200. Weedy
+300. Traditional cultivar / Landrace
+</t>
+  </si>
+  <si>
+    <t>110
+200</t>
+  </si>
+  <si>
+    <t>SAMPSTAT</t>
   </si>
 </sst>
 </file>
@@ -1432,7 +1634,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1579,8 +1781,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1692,8 +1920,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1884,8 +2113,19 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="112">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1943,6 +2183,7 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2296,22 +2537,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AS16"/>
+  <dimension ref="A1:AZ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="AO4" sqref="AO4:AU8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
     <col min="2" max="30" width="39.5" style="5" customWidth="1"/>
-    <col min="31" max="45" width="39.5" customWidth="1"/>
-    <col min="46" max="16384" width="8.83203125" style="6"/>
+    <col min="31" max="52" width="39.5" customWidth="1"/>
+    <col min="53" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="9" customFormat="1" ht="18">
+    <row r="1" spans="1:52" s="9" customFormat="1" ht="18">
       <c r="A1" s="23" t="s">
         <v>14</v>
       </c>
@@ -2358,9 +2599,16 @@
       <c r="AP1" s="24"/>
       <c r="AQ1" s="24"/>
       <c r="AR1" s="24"/>
-      <c r="AS1" s="25"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="25"/>
     </row>
-    <row r="2" spans="1:45" s="11" customFormat="1" ht="15">
+    <row r="2" spans="1:52" s="11" customFormat="1" ht="15">
       <c r="A2" s="26" t="s">
         <v>15</v>
       </c>
@@ -2407,9 +2655,16 @@
       <c r="AP2" s="10"/>
       <c r="AQ2" s="10"/>
       <c r="AR2" s="10"/>
-      <c r="AS2" s="27"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="27"/>
     </row>
-    <row r="3" spans="1:45" s="11" customFormat="1" ht="15">
+    <row r="3" spans="1:52" s="11" customFormat="1" ht="15">
       <c r="A3" s="26"/>
       <c r="B3" s="66"/>
       <c r="C3" s="66"/>
@@ -2454,9 +2709,16 @@
       <c r="AP3" s="10"/>
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
-      <c r="AS3" s="27"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="10"/>
+      <c r="AW3" s="10"/>
+      <c r="AX3" s="10"/>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="27"/>
     </row>
-    <row r="4" spans="1:45" s="12" customFormat="1">
+    <row r="4" spans="1:52" s="12" customFormat="1">
       <c r="A4" s="28" t="s">
         <v>16</v>
       </c>
@@ -2578,22 +2840,43 @@
         <v>122</v>
       </c>
       <c r="AO4" s="43" t="s">
+        <v>335</v>
+      </c>
+      <c r="AP4" s="43" t="s">
+        <v>336</v>
+      </c>
+      <c r="AQ4" s="43" t="s">
+        <v>337</v>
+      </c>
+      <c r="AR4" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="AS4" s="43" t="s">
+        <v>339</v>
+      </c>
+      <c r="AT4" s="43" t="s">
+        <v>340</v>
+      </c>
+      <c r="AU4" s="43" t="s">
+        <v>341</v>
+      </c>
+      <c r="AV4" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="AP4" s="43" t="s">
+      <c r="AW4" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="AQ4" s="43" t="s">
+      <c r="AX4" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="AR4" s="44" t="s">
+      <c r="AY4" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="AS4" s="46" t="s">
+      <c r="AZ4" s="46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:45" s="7" customFormat="1" ht="154">
+    <row r="5" spans="1:52" s="7" customFormat="1" ht="168">
       <c r="A5" s="29" t="s">
         <v>333</v>
       </c>
@@ -2705,22 +2988,43 @@
         <v>123</v>
       </c>
       <c r="AO5" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="AP5" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="AQ5" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="AR5" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="AS5" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="AT5" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="AU5" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="AV5" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="AP5" s="13" t="s">
+      <c r="AW5" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="AQ5" s="13" t="s">
+      <c r="AX5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="AR5" s="13" t="s">
+      <c r="AY5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AS5" s="30" t="s">
+      <c r="AZ5" s="30" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:45" s="8" customFormat="1" ht="70">
+    <row r="6" spans="1:52" s="8" customFormat="1" ht="70">
       <c r="A6" s="31"/>
       <c r="B6" s="69"/>
       <c r="C6" s="69"/>
@@ -2807,15 +3111,36 @@
       </c>
       <c r="AM6" s="22"/>
       <c r="AN6" s="22"/>
-      <c r="AO6" s="22"/>
+      <c r="AO6" s="22" t="s">
+        <v>349</v>
+      </c>
       <c r="AP6" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="AQ6" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="AR6" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="AS6" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT6" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="AU6" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="AV6" s="22"/>
+      <c r="AW6" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="AQ6" s="22"/>
-      <c r="AR6" s="22"/>
-      <c r="AS6" s="32"/>
+      <c r="AX6" s="22"/>
+      <c r="AY6" s="22"/>
+      <c r="AZ6" s="32"/>
     </row>
-    <row r="7" spans="1:45" s="8" customFormat="1">
+    <row r="7" spans="1:52" s="8" customFormat="1">
       <c r="A7" s="33" t="s">
         <v>22</v>
       </c>
@@ -2882,9 +3207,16 @@
       <c r="AP7" s="16"/>
       <c r="AQ7" s="16"/>
       <c r="AR7" s="16"/>
-      <c r="AS7" s="34"/>
+      <c r="AS7" s="16"/>
+      <c r="AT7" s="16"/>
+      <c r="AU7" s="16"/>
+      <c r="AV7" s="16"/>
+      <c r="AW7" s="16"/>
+      <c r="AX7" s="16"/>
+      <c r="AY7" s="16"/>
+      <c r="AZ7" s="34"/>
     </row>
-    <row r="8" spans="1:45" s="8" customFormat="1" ht="15" thickBot="1">
+    <row r="8" spans="1:52" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="A8" s="35" t="s">
         <v>334</v>
       </c>
@@ -3006,22 +3338,43 @@
         <v>121</v>
       </c>
       <c r="AO8" s="37" t="s">
+        <v>354</v>
+      </c>
+      <c r="AP8" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="AQ8" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="AR8" s="37" t="s">
+        <v>357</v>
+      </c>
+      <c r="AS8" s="37" t="s">
+        <v>358</v>
+      </c>
+      <c r="AT8" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="AU8" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="AV8" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="AP8" s="37" t="s">
+      <c r="AW8" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="AQ8" s="37" t="s">
+      <c r="AX8" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="AR8" s="37" t="s">
+      <c r="AY8" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="AS8" s="38" t="s">
+      <c r="AZ8" s="38" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="28">
+    <row r="9" spans="1:52" ht="28">
       <c r="A9" s="57">
         <v>1</v>
       </c>
@@ -3134,23 +3487,30 @@
       <c r="AN9" s="60" t="s">
         <v>286</v>
       </c>
-      <c r="AO9" s="60" t="s">
+      <c r="AO9" s="60"/>
+      <c r="AP9" s="60"/>
+      <c r="AQ9" s="60"/>
+      <c r="AR9" s="60"/>
+      <c r="AS9" s="60"/>
+      <c r="AT9" s="60"/>
+      <c r="AU9" s="60"/>
+      <c r="AV9" s="60" t="s">
         <v>252</v>
       </c>
-      <c r="AP9" s="60">
+      <c r="AW9" s="60">
         <v>30</v>
       </c>
-      <c r="AQ9" s="60" t="s">
+      <c r="AX9" s="60" t="s">
         <v>287</v>
       </c>
-      <c r="AR9" s="60" t="s">
+      <c r="AY9" s="60" t="s">
         <v>288</v>
       </c>
-      <c r="AS9" s="60" t="s">
+      <c r="AZ9" s="60" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:45" ht="28">
+    <row r="10" spans="1:52" ht="28">
       <c r="B10" s="5" t="s">
         <v>237</v>
       </c>
@@ -3259,23 +3619,23 @@
       <c r="AN10" t="s">
         <v>286</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AV10" t="s">
         <v>252</v>
       </c>
-      <c r="AP10">
+      <c r="AW10">
         <v>30</v>
       </c>
-      <c r="AQ10" t="s">
+      <c r="AX10" t="s">
         <v>287</v>
       </c>
-      <c r="AR10" t="s">
+      <c r="AY10" t="s">
         <v>288</v>
       </c>
-      <c r="AS10" t="s">
+      <c r="AZ10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:52">
       <c r="C11" s="50"/>
       <c r="E11" s="51"/>
       <c r="F11"/>
@@ -3290,7 +3650,7 @@
       <c r="AK11" s="5"/>
       <c r="AM11" s="5"/>
     </row>
-    <row r="12" spans="1:45" ht="28">
+    <row r="12" spans="1:52" ht="28">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -3402,23 +3762,23 @@
       <c r="AN12" t="s">
         <v>286</v>
       </c>
-      <c r="AO12" t="s">
+      <c r="AV12" t="s">
         <v>252</v>
       </c>
-      <c r="AP12">
+      <c r="AW12">
         <v>30</v>
       </c>
-      <c r="AQ12" t="s">
+      <c r="AX12" t="s">
         <v>287</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AY12" t="s">
         <v>288</v>
       </c>
-      <c r="AS12" t="s">
+      <c r="AZ12" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="28">
+    <row r="13" spans="1:52" ht="28">
       <c r="A13" s="57">
         <v>4</v>
       </c>
@@ -3531,23 +3891,30 @@
       <c r="AN13" s="60" t="s">
         <v>286</v>
       </c>
-      <c r="AO13" s="60" t="s">
+      <c r="AO13" s="60"/>
+      <c r="AP13" s="60"/>
+      <c r="AQ13" s="60"/>
+      <c r="AR13" s="60"/>
+      <c r="AS13" s="60"/>
+      <c r="AT13" s="60"/>
+      <c r="AU13" s="60"/>
+      <c r="AV13" s="60" t="s">
         <v>252</v>
       </c>
-      <c r="AP13" s="60">
+      <c r="AW13" s="60">
         <v>30</v>
       </c>
-      <c r="AQ13" s="60" t="s">
+      <c r="AX13" s="60" t="s">
         <v>287</v>
       </c>
-      <c r="AR13" s="60" t="s">
+      <c r="AY13" s="60" t="s">
         <v>288</v>
       </c>
-      <c r="AS13" s="60" t="s">
+      <c r="AZ13" s="60" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:45" ht="28">
+    <row r="14" spans="1:52" ht="28">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -3656,23 +4023,23 @@
       <c r="AN14" t="s">
         <v>286</v>
       </c>
-      <c r="AO14" t="s">
+      <c r="AV14" t="s">
         <v>252</v>
       </c>
-      <c r="AP14">
+      <c r="AW14">
         <v>70</v>
       </c>
-      <c r="AQ14" t="s">
+      <c r="AX14" t="s">
         <v>287</v>
       </c>
-      <c r="AR14" t="s">
+      <c r="AY14" t="s">
         <v>288</v>
       </c>
-      <c r="AS14" t="s">
+      <c r="AZ14" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:45" ht="28">
+    <row r="15" spans="1:52" ht="28">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -3766,23 +4133,23 @@
       <c r="AN15" t="s">
         <v>286</v>
       </c>
-      <c r="AO15" t="s">
+      <c r="AV15" t="s">
         <v>252</v>
       </c>
-      <c r="AP15">
+      <c r="AW15">
         <v>70</v>
       </c>
-      <c r="AQ15" t="s">
+      <c r="AX15" t="s">
         <v>287</v>
       </c>
-      <c r="AR15" t="s">
+      <c r="AY15" t="s">
         <v>288</v>
       </c>
-      <c r="AS15" t="s">
+      <c r="AZ15" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:45" ht="28">
+    <row r="16" spans="1:52" ht="28">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -3876,19 +4243,19 @@
       <c r="AN16" t="s">
         <v>286</v>
       </c>
-      <c r="AO16" t="s">
+      <c r="AV16" t="s">
         <v>252</v>
       </c>
-      <c r="AP16">
+      <c r="AW16">
         <v>70</v>
       </c>
-      <c r="AQ16" t="s">
+      <c r="AX16" t="s">
         <v>287</v>
       </c>
-      <c r="AR16" t="s">
+      <c r="AY16" t="s">
         <v>288</v>
       </c>
-      <c r="AS16" t="s">
+      <c r="AZ16" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3927,9 +4294,9 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4202,20 +4569,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39.5" style="1" customWidth="1"/>
-    <col min="2" max="20" width="39.5" style="5" customWidth="1"/>
+    <col min="2" max="23" width="39.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18">
+    <row r="1" spans="1:23" ht="18">
       <c r="A1" s="23" t="s">
         <v>172</v>
       </c>
@@ -4237,9 +4604,12 @@
       <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
       <c r="S1" s="24"/>
-      <c r="T1" s="25"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="25"/>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="15">
+    <row r="2" spans="1:23" s="4" customFormat="1" ht="15">
       <c r="A2" s="26" t="s">
         <v>173</v>
       </c>
@@ -4261,9 +4631,12 @@
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
-      <c r="T2" s="27"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="27"/>
     </row>
-    <row r="3" spans="1:20" s="4" customFormat="1" ht="15">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="15">
       <c r="A3" s="26"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -4283,9 +4656,12 @@
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
-      <c r="T3" s="27"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="27"/>
     </row>
-    <row r="4" spans="1:20" s="47" customFormat="1">
+    <row r="4" spans="1:23" s="47" customFormat="1">
       <c r="A4" s="28" t="s">
         <v>16</v>
       </c>
@@ -4296,58 +4672,67 @@
         <v>179</v>
       </c>
       <c r="D4" s="43" t="s">
+        <v>361</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>362</v>
+      </c>
+      <c r="F4" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="G4" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="H4" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="I4" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="J4" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="K4" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="L4" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="M4" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="L4" s="43" t="s">
+      <c r="N4" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="O4" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="P4" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="O4" s="43" t="s">
+      <c r="Q4" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="R4" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="Q4" s="43" t="s">
+      <c r="S4" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="T4" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="S4" s="43" t="s">
+      <c r="U4" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="T4" s="48" t="s">
+      <c r="V4" s="74" t="s">
+        <v>374</v>
+      </c>
+      <c r="W4" s="48" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="4" customFormat="1" ht="224">
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="224">
       <c r="A5" s="29" t="s">
         <v>174</v>
       </c>
@@ -4358,94 +4743,112 @@
         <v>10</v>
       </c>
       <c r="D5" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="G5" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="H5" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="I5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="J5" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="K5" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="L5" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="M5" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="N5" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="O5" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="P5" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="Q5" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="R5" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="Q5" s="13" t="s">
+      <c r="S5" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="T5" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="U5" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="T5" s="30" t="s">
+      <c r="V5" s="75" t="s">
+        <v>375</v>
+      </c>
+      <c r="W5" s="30" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="4" customFormat="1">
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="42">
       <c r="A6" s="31"/>
       <c r="B6" s="14" t="s">
         <v>178</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="G6" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
+      <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
-      <c r="S6" s="15" t="s">
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="T6" s="49"/>
+      <c r="V6" s="78" t="s">
+        <v>376</v>
+      </c>
+      <c r="W6" s="49"/>
     </row>
-    <row r="7" spans="1:20" s="4" customFormat="1">
+    <row r="7" spans="1:23" s="4" customFormat="1">
       <c r="A7" s="33" t="s">
         <v>22</v>
       </c>
@@ -4457,21 +4860,24 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="16"/>
       <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="O7" s="17"/>
       <c r="P7" s="16"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
-      <c r="S7" s="16" t="s">
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="T7" s="34"/>
+      <c r="V7" s="76"/>
+      <c r="W7" s="34"/>
     </row>
-    <row r="8" spans="1:20" s="3" customFormat="1" ht="15" thickBot="1">
+    <row r="8" spans="1:23" s="3" customFormat="1" ht="15" thickBot="1">
       <c r="A8" s="73" t="s">
         <v>334</v>
       </c>
@@ -4482,58 +4888,67 @@
         <v>180</v>
       </c>
       <c r="D8" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>368</v>
+      </c>
+      <c r="F8" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="G8" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="H8" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="I8" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="J8" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="K8" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="L8" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="K8" s="36" t="s">
+      <c r="M8" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="L8" s="36" t="s">
+      <c r="N8" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="O8" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="N8" s="36" t="s">
+      <c r="P8" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="Q8" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="P8" s="36" t="s">
+      <c r="R8" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="Q8" s="36" t="s">
+      <c r="S8" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="R8" s="37" t="s">
+      <c r="T8" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="S8" s="37" t="s">
+      <c r="U8" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="T8" s="38" t="s">
+      <c r="V8" s="77" t="s">
+        <v>377</v>
+      </c>
+      <c r="W8" s="38" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:23">
       <c r="A9" s="57">
         <v>1</v>
       </c>
@@ -4544,58 +4959,67 @@
         <v>255</v>
       </c>
       <c r="D9" s="58" t="s">
+        <v>290</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>369</v>
+      </c>
+      <c r="F9" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="G9" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="H9" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="I9" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="J9" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="I9" s="58">
+      <c r="K9" s="58">
         <v>2</v>
       </c>
-      <c r="J9" s="58">
+      <c r="L9" s="58">
         <v>2015</v>
       </c>
-      <c r="K9" s="59" t="s">
+      <c r="M9" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="L9" s="58" t="s">
+      <c r="N9" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="M9" s="58" t="s">
+      <c r="O9" s="58" t="s">
         <v>260</v>
       </c>
-      <c r="N9" s="58" t="s">
+      <c r="P9" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="O9" s="58" t="s">
+      <c r="Q9" s="58" t="s">
         <v>313</v>
       </c>
-      <c r="P9" s="58" t="s">
+      <c r="R9" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="Q9" s="58" t="s">
+      <c r="S9" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="R9" s="58">
+      <c r="T9" s="58">
         <v>1987</v>
       </c>
-      <c r="S9" s="58">
+      <c r="U9" s="58">
         <v>100</v>
       </c>
-      <c r="T9" s="58" t="s">
+      <c r="V9" s="58">
+        <v>110</v>
+      </c>
+      <c r="W9" s="58" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:23">
       <c r="A10" s="57">
         <v>1</v>
       </c>
@@ -4606,58 +5030,67 @@
         <v>263</v>
       </c>
       <c r="D10" s="58" t="s">
+        <v>290</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="G10" s="58" t="s">
         <v>317</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="H10" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="I10" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="J10" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="I10" s="58">
+      <c r="K10" s="58">
         <v>3</v>
       </c>
-      <c r="J10" s="58">
+      <c r="L10" s="58">
         <v>2015</v>
       </c>
-      <c r="K10" s="59" t="s">
+      <c r="M10" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="L10" s="58" t="s">
+      <c r="N10" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="M10" s="58" t="s">
+      <c r="O10" s="58" t="s">
         <v>260</v>
       </c>
-      <c r="N10" s="58" t="s">
+      <c r="P10" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="O10" s="58" t="s">
+      <c r="Q10" s="58" t="s">
         <v>313</v>
       </c>
-      <c r="P10" s="58" t="s">
+      <c r="R10" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="Q10" s="58" t="s">
+      <c r="S10" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="R10" s="58">
+      <c r="T10" s="58">
         <v>1987</v>
       </c>
-      <c r="S10" s="58">
+      <c r="U10" s="58">
         <v>410</v>
       </c>
-      <c r="T10" s="58" t="s">
+      <c r="V10" s="58">
+        <v>120</v>
+      </c>
+      <c r="W10" s="58" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:23">
       <c r="A11" s="57">
         <v>4</v>
       </c>
@@ -4668,58 +5101,67 @@
         <v>265</v>
       </c>
       <c r="D11" s="58" t="s">
+        <v>370</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>371</v>
+      </c>
+      <c r="F11" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="G11" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="H11" s="58" t="s">
         <v>315</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="I11" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="J11" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="I11" s="58">
+      <c r="K11" s="58">
         <v>3</v>
       </c>
-      <c r="J11" s="58">
+      <c r="L11" s="58">
         <v>2015</v>
       </c>
-      <c r="K11" s="59" t="s">
+      <c r="M11" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="N11" s="58" t="s">
         <v>316</v>
       </c>
-      <c r="M11" s="58" t="s">
+      <c r="O11" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="N11" s="58" t="s">
+      <c r="P11" s="58" t="s">
         <v>317</v>
       </c>
-      <c r="O11" s="58" t="s">
+      <c r="Q11" s="58" t="s">
         <v>313</v>
       </c>
-      <c r="P11" s="58" t="s">
+      <c r="R11" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="Q11" s="58" t="s">
+      <c r="S11" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="R11" s="58">
+      <c r="T11" s="58">
         <v>1977</v>
       </c>
-      <c r="S11" s="58">
+      <c r="U11" s="58">
         <v>410</v>
       </c>
-      <c r="T11" s="58" t="s">
+      <c r="V11" s="58">
+        <v>100</v>
+      </c>
+      <c r="W11" s="58" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:23">
       <c r="A12" s="57">
         <v>4</v>
       </c>
@@ -4730,54 +5172,63 @@
         <v>324</v>
       </c>
       <c r="D12" s="58" t="s">
+        <v>372</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>373</v>
+      </c>
+      <c r="F12" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="G12" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="H12" s="58" t="s">
         <v>315</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="I12" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="H12" s="58" t="s">
+      <c r="J12" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="I12" s="58">
+      <c r="K12" s="58">
         <v>3</v>
       </c>
-      <c r="J12" s="58"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="58" t="s">
+      <c r="L12" s="58"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="58" t="s">
         <v>316</v>
       </c>
-      <c r="M12" s="58" t="s">
+      <c r="O12" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="N12" s="58" t="s">
+      <c r="P12" s="58" t="s">
         <v>317</v>
       </c>
-      <c r="O12" s="58" t="s">
+      <c r="Q12" s="58" t="s">
         <v>313</v>
       </c>
-      <c r="P12" s="58" t="s">
+      <c r="R12" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="Q12" s="58" t="s">
+      <c r="S12" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="R12" s="58">
+      <c r="T12" s="58">
         <v>1977</v>
       </c>
-      <c r="S12" s="58">
+      <c r="U12" s="58">
         <v>410</v>
       </c>
-      <c r="T12" s="58" t="s">
+      <c r="V12" s="58">
+        <v>200</v>
+      </c>
+      <c r="W12" s="58" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:23">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -4798,8 +5249,11 @@
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:23">
       <c r="A14" s="1">
         <v>999</v>
       </c>
@@ -4810,34 +5264,43 @@
         <v>265</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="I14" s="5">
+      <c r="K14" s="5">
         <v>3</v>
       </c>
-      <c r="J14" s="5">
+      <c r="L14" s="5">
         <v>2015</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="O14" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="S14" s="5">
+      <c r="U14" s="5">
         <v>410</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="V14" s="5">
+        <v>300</v>
+      </c>
+      <c r="W14" s="5" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:23">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -4848,34 +5311,40 @@
         <v>265</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="I15" s="5">
+      <c r="K15" s="5">
         <v>4</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="M15" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="O15" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="S15" s="5" t="s">
+      <c r="U15" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="T15" s="5" t="s">
+      <c r="W15" s="5" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:23">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -4886,31 +5355,40 @@
         <v>265</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="I16" s="5">
+      <c r="K16" s="5">
         <v>4</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="O16" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="T16" s="5" t="s">
+      <c r="V16" s="5">
+        <v>200</v>
+      </c>
+      <c r="W16" s="5" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="17" spans="2:20">
+    <row r="17" spans="2:23">
       <c r="B17" s="5">
         <v>4</v>
       </c>
@@ -4918,38 +5396,44 @@
         <v>265</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="I17" s="5">
+      <c r="K17" s="5">
         <v>4</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="O17" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="S17" s="5" t="s">
+      <c r="U17" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="T17" s="5" t="s">
+      <c r="W17" s="5" t="s">
         <v>325</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K9" r:id="rId1"/>
-    <hyperlink ref="K11" r:id="rId2"/>
-    <hyperlink ref="K10" r:id="rId3"/>
+    <hyperlink ref="M9" r:id="rId1"/>
+    <hyperlink ref="M11" r:id="rId2"/>
+    <hyperlink ref="M10" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0"/>

</xml_diff>